<commit_message>
Fix: Fixed DDL output processing.
</commit_message>
<xml_diff>
--- a/gen/properties_list.xlsx
+++ b/gen/properties_list.xlsx
@@ -169,12 +169,6 @@
     <t>テーブル名にスキーマを付与する</t>
   </si>
   <si>
-    <t>wizard.generate.ddl.dropTable</t>
-  </si>
-  <si>
-    <t>DROP TABLE文を出力する</t>
-  </si>
-  <si>
     <t>wizard.generate.ddl.alterTable</t>
   </si>
   <si>
@@ -1430,9 +1424,6 @@
   </si>
   <si>
     <t>With schema name</t>
-  </si>
-  <si>
-    <t>With DROP TABLE statement</t>
   </si>
   <si>
     <t>Generates constraints as ALTER TABLE</t>
@@ -2100,6 +2091,18 @@
   </si>
   <si>
     <t>validation.error.noPrimaryKey</t>
+  </si>
+  <si>
+    <t>DROP文を出力する</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>With DROP statement</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wizard.generate.ddl.drop</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -2531,2242 +2534,2242 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A102" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A106" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A121" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="B124" s="2"/>
       <c r="C124" s="1"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A135" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A137" s="1" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A142" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A143" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A144" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A145" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A146" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A147" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A148" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A149" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A150" s="1" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A151" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A152" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A153" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A154" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A155" s="1" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A156" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A157" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A158" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A159" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A160" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A161" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A162" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A163" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A164" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A165" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A166" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A167" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A168" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A169" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A170" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A171" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A172" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A173" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A174" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A175" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A176" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A177" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A178" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A179" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A180" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A181" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A182" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A183" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A184" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A185" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A186" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A187" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A188" s="1" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A189" s="1" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A190" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A191" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A192" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A193" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A194" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A195" s="1" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A196" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A197" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A198" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A199" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A200" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A201" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A202" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A203" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A204" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A205" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.15">
@@ -4774,7 +4777,7 @@
         <v>39</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>40</v>
@@ -4785,7 +4788,7 @@
         <v>37</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>38</v>
@@ -4793,35 +4796,35 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A208" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A209" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A210" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.15">
@@ -4829,7 +4832,7 @@
         <v>43</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>44</v>
@@ -4837,13 +4840,13 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A212" s="1" t="s">
-        <v>51</v>
+        <v>684</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>472</v>
+        <v>683</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>52</v>
+        <v>682</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.15">
@@ -4851,7 +4854,7 @@
         <v>47</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>48</v>
@@ -4859,46 +4862,46 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A214" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A215" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A216" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A217" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.15">
@@ -4906,7 +4909,7 @@
         <v>45</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>46</v>
@@ -4917,7 +4920,7 @@
         <v>49</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>50</v>
@@ -4939,7 +4942,7 @@
         <v>35</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>36</v>
@@ -4947,32 +4950,32 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A222" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A223" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A224" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>11</v>
@@ -4980,13 +4983,13 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A225" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.15">
@@ -4994,7 +4997,7 @@
         <v>6</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>7</v>
@@ -5005,7 +5008,7 @@
         <v>2</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>3</v>
@@ -5016,7 +5019,7 @@
         <v>4</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>5</v>
@@ -5027,7 +5030,7 @@
         <v>0</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C229" s="1" t="s">
         <v>1</v>
@@ -5038,7 +5041,7 @@
         <v>33</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>34</v>
@@ -5049,7 +5052,7 @@
         <v>21</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>22</v>
@@ -5060,7 +5063,7 @@
         <v>12</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>13</v>
@@ -5071,7 +5074,7 @@
         <v>29</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>30</v>
@@ -5082,7 +5085,7 @@
         <v>31</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>32</v>
@@ -5093,7 +5096,7 @@
         <v>25</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>26</v>
@@ -5104,7 +5107,7 @@
         <v>10</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>11</v>
@@ -5115,7 +5118,7 @@
         <v>18</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>19</v>
@@ -5126,7 +5129,7 @@
         <v>20</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>5</v>
@@ -5137,7 +5140,7 @@
         <v>27</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>28</v>
@@ -5148,7 +5151,7 @@
         <v>8</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>9</v>
@@ -5159,7 +5162,7 @@
         <v>14</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>15</v>
@@ -5170,7 +5173,7 @@
         <v>16</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>17</v>
@@ -5181,7 +5184,7 @@
         <v>23</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Work: Update the HTML generator
</commit_message>
<xml_diff>
--- a/gen/properties_list.xlsx
+++ b/gen/properties_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="757">
   <si>
     <t>wizard.new.erd.title</t>
   </si>
@@ -2117,6 +2117,285 @@
     <t>改行コード:</t>
     <rPh sb="0" eb="2">
       <t>カイギョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テーブル定義</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>論理テーブル名</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>論理テーブル名</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>説明</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>No.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>論理名</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>物理名</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>型</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>必須</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>一意</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>符号無し</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>初期値</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>備考</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ドメイン</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>インデックス</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>外部キー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ドメイン定義</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ドメイン名</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>型</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サイズ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>このテーブルを参照しているテーブル</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.title</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.table.logicalName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.table.physicalName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.table.description</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.column.rownum</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.column.logicalName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.column.physicalName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.column.type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.column.notNull</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.column.unique</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>htmlcolumn.unsigned</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.column.defaultValue</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.column.description</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.column.description.domain</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.indices</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.foreignKeys</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.domain.title</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.domain.name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.domain.type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.domain.size</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.referencedTables</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>note.importedTable</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※このテーブルは他のダイアグラムからインポートされたテーブルです。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Tables</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Logical Table Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Unique</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Unsigned</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Domain Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Physical Table Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>No.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.column.primaryKey</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PrimaryKey</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Logical Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Physical Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Not Null</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Default Value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Domain</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Indices</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Foreign Keys</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Domain Definitions</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Size</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Referenced Tables</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Note: This table is imported from other diagram.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>主キー</t>
+    <rPh sb="0" eb="1">
+      <t>シュ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -2236,10 +2515,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="テーブル2" displayName="テーブル2" ref="A2:C244" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A2:C244"/>
-  <sortState ref="A3:C244">
-    <sortCondition ref="A2:A244"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="テーブル2" displayName="テーブル2" ref="A2:C267" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A2:C267"/>
+  <sortState ref="A3:C267">
+    <sortCondition ref="A2:A267"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="2" name="Key" dataDxfId="2"/>
@@ -2537,9 +2816,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C244"/>
+  <dimension ref="A2:C267"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3705,1515 +3986,1768 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>373</v>
+        <v>720</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>670</v>
+        <v>748</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>669</v>
+        <v>699</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
-        <v>665</v>
+        <v>721</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>666</v>
+        <v>734</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>376</v>
+        <v>700</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>397</v>
+        <v>722</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>571</v>
+        <v>749</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>281</v>
+        <v>701</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>379</v>
+        <v>714</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>617</v>
+        <v>744</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>380</v>
+        <v>693</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
-        <v>667</v>
+        <v>717</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>668</v>
+        <v>747</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>378</v>
+        <v>696</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
-        <v>381</v>
+        <v>715</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>581</v>
+        <v>745</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>303</v>
+        <v>694</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
-        <v>382</v>
+        <v>742</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>618</v>
+        <v>743</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>383</v>
+        <v>756</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>391</v>
+        <v>713</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>621</v>
+        <v>741</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>392</v>
+        <v>692</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
-        <v>386</v>
+        <v>716</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>558</v>
+        <v>746</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>250</v>
+        <v>695</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>387</v>
+        <v>718</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>619</v>
+        <v>736</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>388</v>
+        <v>697</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
-        <v>395</v>
+        <v>726</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>623</v>
+        <v>738</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>396</v>
+        <v>705</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
-        <v>393</v>
+        <v>728</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>622</v>
+        <v>753</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>394</v>
+        <v>707</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
-        <v>384</v>
+        <v>725</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>385</v>
+        <v>752</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>385</v>
+        <v>704</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
-        <v>377</v>
+        <v>727</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>482</v>
+        <v>735</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>80</v>
+        <v>706</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A121" s="1" t="s">
-        <v>374</v>
+        <v>724</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>616</v>
+        <v>751</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>375</v>
+        <v>703</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>389</v>
+        <v>723</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>620</v>
+        <v>750</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>390</v>
+        <v>702</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>413</v>
+        <v>729</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>632</v>
+        <v>754</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>414</v>
+        <v>708</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="B124" s="2"/>
-      <c r="C124" s="1"/>
+        <v>712</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
-        <v>83</v>
+        <v>710</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>484</v>
+        <v>733</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>84</v>
+        <v>689</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>85</v>
+        <v>711</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>485</v>
+        <v>739</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>86</v>
+        <v>690</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
-        <v>81</v>
+        <v>709</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>483</v>
+        <v>732</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>82</v>
+        <v>688</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
-        <v>79</v>
+        <v>719</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>482</v>
+        <v>737</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>80</v>
+        <v>698</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
-        <v>77</v>
+        <v>373</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>78</v>
+        <v>670</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>78</v>
+        <v>669</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>357</v>
+        <v>665</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>608</v>
+        <v>666</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>358</v>
+        <v>376</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
-        <v>359</v>
+        <v>397</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>609</v>
+        <v>571</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>360</v>
+        <v>281</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
-        <v>347</v>
+        <v>379</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>603</v>
+        <v>617</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>348</v>
+        <v>380</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
-        <v>351</v>
+        <v>667</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>605</v>
+        <v>668</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>352</v>
+        <v>378</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
-        <v>353</v>
+        <v>381</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>606</v>
+        <v>581</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>354</v>
+        <v>303</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A135" s="1" t="s">
-        <v>349</v>
+        <v>382</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>604</v>
+        <v>618</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>350</v>
+        <v>383</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
-        <v>355</v>
+        <v>391</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>607</v>
+        <v>621</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>356</v>
+        <v>392</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A137" s="1" t="s">
-        <v>649</v>
+        <v>386</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>587</v>
+        <v>558</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>320</v>
+        <v>250</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
-        <v>331</v>
+        <v>387</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>593</v>
+        <v>619</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>332</v>
+        <v>388</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>329</v>
+        <v>395</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>592</v>
+        <v>623</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>330</v>
+        <v>396</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
-        <v>674</v>
+        <v>393</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>599</v>
+        <v>622</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>341</v>
+        <v>394</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
-        <v>675</v>
+        <v>384</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>598</v>
+        <v>385</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>340</v>
+        <v>385</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A142" s="1" t="s">
-        <v>342</v>
+        <v>377</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>600</v>
+        <v>482</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>343</v>
+        <v>80</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A143" s="1" t="s">
-        <v>345</v>
+        <v>374</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>602</v>
+        <v>616</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>346</v>
+        <v>375</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A144" s="1" t="s">
-        <v>344</v>
+        <v>389</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>601</v>
+        <v>620</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>212</v>
+        <v>390</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A145" s="1" t="s">
-        <v>335</v>
+        <v>413</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>595</v>
+        <v>632</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>336</v>
+        <v>414</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A146" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>594</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>334</v>
-      </c>
+        <v>648</v>
+      </c>
+      <c r="B146" s="2"/>
+      <c r="C146" s="1"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A147" s="1" t="s">
-        <v>327</v>
+        <v>730</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>591</v>
+        <v>755</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>328</v>
+        <v>731</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A148" s="1" t="s">
-        <v>325</v>
+        <v>83</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>590</v>
+        <v>484</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>326</v>
+        <v>84</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A149" s="1" t="s">
-        <v>337</v>
+        <v>85</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>596</v>
+        <v>485</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>338</v>
+        <v>86</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A150" s="1" t="s">
-        <v>676</v>
+        <v>81</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>597</v>
+        <v>483</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>339</v>
+        <v>82</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A151" s="1" t="s">
-        <v>323</v>
+        <v>79</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>589</v>
+        <v>482</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>324</v>
+        <v>80</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A152" s="1" t="s">
-        <v>321</v>
+        <v>77</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>588</v>
+        <v>78</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>322</v>
+        <v>78</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A153" s="1" t="s">
-        <v>200</v>
+        <v>357</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>537</v>
+        <v>608</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>201</v>
+        <v>358</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A154" s="1" t="s">
-        <v>203</v>
+        <v>359</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>538</v>
+        <v>609</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>204</v>
+        <v>360</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A155" s="1" t="s">
-        <v>677</v>
+        <v>347</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>534</v>
+        <v>603</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>195</v>
+        <v>348</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A156" s="1" t="s">
-        <v>198</v>
+        <v>351</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>536</v>
+        <v>605</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>199</v>
+        <v>352</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A157" s="1" t="s">
-        <v>193</v>
+        <v>353</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>533</v>
+        <v>606</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>194</v>
+        <v>354</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A158" s="1" t="s">
-        <v>191</v>
+        <v>349</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>532</v>
+        <v>604</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>192</v>
+        <v>350</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A159" s="1" t="s">
-        <v>196</v>
+        <v>355</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>535</v>
+        <v>607</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>197</v>
+        <v>356</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A160" s="1" t="s">
-        <v>202</v>
+        <v>649</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>504</v>
+        <v>587</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>126</v>
+        <v>320</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A161" s="1" t="s">
-        <v>93</v>
+        <v>331</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>489</v>
+        <v>593</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>94</v>
+        <v>332</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A162" s="1" t="s">
-        <v>111</v>
+        <v>329</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>498</v>
+        <v>592</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>112</v>
+        <v>330</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A163" s="1" t="s">
-        <v>105</v>
+        <v>674</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>495</v>
+        <v>599</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>106</v>
+        <v>341</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A164" s="1" t="s">
-        <v>97</v>
+        <v>675</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>491</v>
+        <v>598</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>98</v>
+        <v>340</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A165" s="1" t="s">
-        <v>99</v>
+        <v>342</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>492</v>
+        <v>600</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>100</v>
+        <v>343</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A166" s="1" t="s">
-        <v>101</v>
+        <v>345</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>493</v>
+        <v>602</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>102</v>
+        <v>346</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A167" s="1" t="s">
-        <v>127</v>
+        <v>344</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>128</v>
+        <v>601</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>128</v>
+        <v>212</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A168" s="1" t="s">
-        <v>87</v>
+        <v>335</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>486</v>
+        <v>595</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>88</v>
+        <v>336</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A169" s="1" t="s">
-        <v>119</v>
+        <v>333</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>501</v>
+        <v>594</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>120</v>
+        <v>334</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A170" s="1" t="s">
-        <v>133</v>
+        <v>327</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>507</v>
+        <v>591</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>134</v>
+        <v>328</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A171" s="1" t="s">
-        <v>129</v>
+        <v>325</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>505</v>
+        <v>590</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>130</v>
+        <v>326</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A172" s="1" t="s">
-        <v>135</v>
+        <v>337</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>508</v>
+        <v>596</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>136</v>
+        <v>338</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A173" s="1" t="s">
-        <v>131</v>
+        <v>676</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>506</v>
+        <v>597</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>132</v>
+        <v>339</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A174" s="1" t="s">
-        <v>139</v>
+        <v>323</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>510</v>
+        <v>589</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>140</v>
+        <v>324</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A175" s="1" t="s">
-        <v>137</v>
+        <v>321</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>509</v>
+        <v>588</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>138</v>
+        <v>322</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A176" s="1" t="s">
-        <v>91</v>
+        <v>200</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>488</v>
+        <v>537</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>92</v>
+        <v>201</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A177" s="1" t="s">
-        <v>107</v>
+        <v>203</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>496</v>
+        <v>538</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>108</v>
+        <v>204</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A178" s="1" t="s">
-        <v>109</v>
+        <v>677</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>497</v>
+        <v>534</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>110</v>
+        <v>195</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A179" s="1" t="s">
-        <v>89</v>
+        <v>198</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>487</v>
+        <v>536</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>90</v>
+        <v>199</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A180" s="1" t="s">
-        <v>115</v>
+        <v>193</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>500</v>
+        <v>533</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>116</v>
+        <v>194</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A181" s="1" t="s">
-        <v>95</v>
+        <v>191</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>490</v>
+        <v>532</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>96</v>
+        <v>192</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A182" s="1" t="s">
-        <v>125</v>
+        <v>196</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>504</v>
+        <v>535</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>126</v>
+        <v>197</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A183" s="1" t="s">
-        <v>103</v>
+        <v>202</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>494</v>
+        <v>504</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A184" s="1" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A185" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A186" s="1" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>118</v>
+        <v>495</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A187" s="1" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A188" s="1" t="s">
-        <v>678</v>
+        <v>99</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>643</v>
+        <v>492</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>435</v>
+        <v>100</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A189" s="1" t="s">
-        <v>679</v>
+        <v>101</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>642</v>
+        <v>493</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>434</v>
+        <v>102</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A190" s="1" t="s">
-        <v>431</v>
+        <v>127</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>640</v>
+        <v>128</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>432</v>
+        <v>128</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A191" s="1" t="s">
-        <v>429</v>
+        <v>87</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>639</v>
+        <v>486</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>430</v>
+        <v>88</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A192" s="1" t="s">
-        <v>421</v>
+        <v>119</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>636</v>
+        <v>501</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>422</v>
+        <v>120</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A193" s="1" t="s">
-        <v>419</v>
+        <v>133</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>635</v>
+        <v>507</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>420</v>
+        <v>134</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A194" s="1" t="s">
-        <v>423</v>
+        <v>129</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>637</v>
+        <v>505</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>424</v>
+        <v>130</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A195" s="1" t="s">
-        <v>680</v>
+        <v>135</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>641</v>
+        <v>508</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>433</v>
+        <v>136</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A196" s="1" t="s">
-        <v>438</v>
+        <v>131</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>645</v>
+        <v>506</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>439</v>
+        <v>132</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A197" s="1" t="s">
-        <v>440</v>
+        <v>139</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>646</v>
+        <v>510</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>441</v>
+        <v>140</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A198" s="1" t="s">
-        <v>436</v>
+        <v>137</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>644</v>
+        <v>509</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>437</v>
+        <v>138</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A199" s="1" t="s">
-        <v>427</v>
+        <v>91</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>638</v>
+        <v>488</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>428</v>
+        <v>92</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A200" s="1" t="s">
-        <v>425</v>
+        <v>107</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>671</v>
+        <v>496</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>426</v>
+        <v>108</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A201" s="1" t="s">
-        <v>417</v>
+        <v>109</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>634</v>
+        <v>497</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>418</v>
+        <v>110</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A202" s="1" t="s">
-        <v>415</v>
+        <v>89</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>633</v>
+        <v>487</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>416</v>
+        <v>90</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A203" s="1" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>481</v>
+        <v>500</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A204" s="1" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>480</v>
+        <v>490</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A205" s="1" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>657</v>
+        <v>504</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A206" s="1" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>464</v>
+        <v>494</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A207" s="1" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>463</v>
+        <v>502</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>38</v>
+        <v>122</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A208" s="1" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>469</v>
+        <v>503</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>51</v>
+        <v>124</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A209" s="1" t="s">
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>470</v>
+        <v>118</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A210" s="1" t="s">
-        <v>54</v>
+        <v>113</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>471</v>
+        <v>499</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A211" s="1" t="s">
-        <v>43</v>
+        <v>678</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>465</v>
+        <v>643</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>44</v>
+        <v>435</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A212" s="1" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>682</v>
+        <v>642</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>681</v>
+        <v>434</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A213" s="1" t="s">
-        <v>46</v>
+        <v>431</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>467</v>
+        <v>640</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>47</v>
+        <v>432</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A214" s="1" t="s">
-        <v>60</v>
+        <v>429</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>474</v>
+        <v>639</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>61</v>
+        <v>430</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A215" s="1" t="s">
-        <v>58</v>
+        <v>421</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>473</v>
+        <v>636</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>59</v>
+        <v>422</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A216" s="1" t="s">
-        <v>62</v>
+        <v>419</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>475</v>
+        <v>635</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>63</v>
+        <v>420</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A217" s="1" t="s">
-        <v>56</v>
+        <v>423</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>472</v>
+        <v>637</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>57</v>
+        <v>424</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A218" s="1" t="s">
-        <v>45</v>
+        <v>680</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>466</v>
+        <v>641</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>686</v>
+        <v>433</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A219" s="1" t="s">
-        <v>684</v>
+        <v>438</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>685</v>
+        <v>645</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>687</v>
+        <v>439</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A220" s="1" t="s">
-        <v>48</v>
+        <v>440</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>468</v>
+        <v>646</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>49</v>
+        <v>441</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A221" s="1" t="s">
-        <v>41</v>
+        <v>436</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>42</v>
+        <v>644</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>42</v>
+        <v>437</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A222" s="1" t="s">
-        <v>35</v>
+        <v>427</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>462</v>
+        <v>638</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>36</v>
+        <v>428</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A223" s="1" t="s">
-        <v>67</v>
+        <v>425</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>477</v>
+        <v>671</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>68</v>
+        <v>426</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A224" s="1" t="s">
-        <v>69</v>
+        <v>417</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>478</v>
+        <v>634</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>70</v>
+        <v>418</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A225" s="1" t="s">
-        <v>66</v>
+        <v>415</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>449</v>
+        <v>633</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>11</v>
+        <v>416</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A226" s="1" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A227" s="1" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>447</v>
+        <v>480</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A228" s="1" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>445</v>
+        <v>657</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A229" s="1" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>446</v>
+        <v>464</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A230" s="1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>444</v>
+        <v>463</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A231" s="1" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A232" s="1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>455</v>
+        <v>470</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A233" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>450</v>
+        <v>471</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A234" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>459</v>
+        <v>465</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A235" s="1" t="s">
-        <v>31</v>
+        <v>683</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>460</v>
+        <v>682</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>32</v>
+        <v>681</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A236" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A237" s="1" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>449</v>
+        <v>474</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A238" s="1" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>453</v>
+        <v>473</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A239" s="1" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>454</v>
+        <v>475</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A240" s="1" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>458</v>
+        <v>472</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A241" s="1" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>448</v>
+        <v>466</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>9</v>
+        <v>686</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A242" s="1" t="s">
-        <v>14</v>
+        <v>684</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>451</v>
+        <v>685</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>15</v>
+        <v>687</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A243" s="1" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>452</v>
+        <v>468</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A244" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A245" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A246" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A247" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A248" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A249" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A250" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A251" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A252" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A254" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A255" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A256" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A257" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A258" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A259" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A260" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A261" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A262" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A263" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A264" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A265" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A266" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A267" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B244" s="1" t="s">
+      <c r="B267" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="C244" s="1" t="s">
+      <c r="C267" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FIX: Fixed a bug in the HTML generator output.
</commit_message>
<xml_diff>
--- a/gen/properties_list.xlsx
+++ b/gen/properties_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="775">
   <si>
     <t>wizard.new.erd.title</t>
   </si>
@@ -2205,10 +2205,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>html.title</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>html.table.logicalName</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -2237,19 +2233,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>html.column.notNull</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>html.column.unique</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>htmlcolumn.unsigned</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.column.defaultValue</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -2397,6 +2381,109 @@
     <rPh sb="0" eb="1">
       <t>シュ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Table</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テーブル</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Attribute Overview</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>属性の概要</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>外部キー</t>
+    <rPh sb="0" eb="2">
+      <t>ガイブ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.title</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.page.section.title.index</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Indexing Overview</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>インデックスの概要</t>
+    <rPh sb="7" eb="9">
+      <t>ガイヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.page.section.title.attribute</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.page.title.table</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.column.unsigned</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>複合一意キー</t>
+    <rPh sb="0" eb="2">
+      <t>フクゴウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>イチイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.page.section.title.compositeUniqueKeys</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Composite Unique Keys</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Foreign Keys</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.page.section.title.foreignKeys</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.column.defaultValue</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Auto Increment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>自動採番</t>
+    <rPh sb="2" eb="4">
+      <t>サイバン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.column.autoIncrement</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>html.column.notNull</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2515,10 +2602,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="テーブル2" displayName="テーブル2" ref="A2:C267" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A2:C267"/>
-  <sortState ref="A3:C267">
-    <sortCondition ref="A2:A267"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="テーブル2" displayName="テーブル2" ref="A2:C273" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A2:C273"/>
+  <sortState ref="A3:C273">
+    <sortCondition ref="A2:A273"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="2" name="Key" dataDxfId="2"/>
@@ -2816,11 +2903,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C267"/>
+  <dimension ref="A2:C273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3986,167 +4071,167 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>720</v>
+        <v>773</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>748</v>
+        <v>771</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>699</v>
+        <v>772</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
-        <v>721</v>
+        <v>770</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>734</v>
+        <v>744</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>749</v>
+        <v>730</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>693</v>
+        <v>701</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>747</v>
+        <v>740</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
-        <v>715</v>
+        <v>774</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
-        <v>742</v>
+        <v>714</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>756</v>
+        <v>694</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>713</v>
+        <v>738</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>692</v>
+        <v>752</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>746</v>
+        <v>737</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>736</v>
+        <v>742</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
-        <v>726</v>
+        <v>716</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
-        <v>728</v>
+        <v>764</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>753</v>
+        <v>733</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>707</v>
+        <v>698</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>752</v>
+        <v>734</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>735</v>
+        <v>749</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A121" s="1" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.15">
@@ -4154,1600 +4239,1666 @@
         <v>723</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>750</v>
+        <v>731</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>729</v>
+        <v>720</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>754</v>
+        <v>747</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
-        <v>712</v>
+        <v>719</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>740</v>
+        <v>746</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>691</v>
+        <v>702</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
-        <v>710</v>
+        <v>762</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>733</v>
+        <v>755</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>689</v>
+        <v>756</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>711</v>
+        <v>766</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>739</v>
+        <v>767</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>690</v>
+        <v>765</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
-        <v>709</v>
+        <v>769</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>732</v>
+        <v>768</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>688</v>
+        <v>757</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
-        <v>719</v>
+        <v>759</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>737</v>
+        <v>760</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>698</v>
+        <v>761</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
-        <v>373</v>
+        <v>763</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>670</v>
+        <v>753</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>669</v>
+        <v>754</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>665</v>
+        <v>725</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>666</v>
+        <v>750</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>376</v>
+        <v>708</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
-        <v>397</v>
+        <v>711</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>571</v>
+        <v>736</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>281</v>
+        <v>691</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
-        <v>379</v>
+        <v>709</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>617</v>
+        <v>729</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>380</v>
+        <v>689</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
-        <v>667</v>
+        <v>710</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>668</v>
+        <v>735</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>378</v>
+        <v>690</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
-        <v>381</v>
+        <v>758</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>581</v>
+        <v>728</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>303</v>
+        <v>688</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A135" s="1" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>618</v>
+        <v>670</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>383</v>
+        <v>669</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
-        <v>391</v>
+        <v>665</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>621</v>
+        <v>666</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A137" s="1" t="s">
-        <v>386</v>
+        <v>397</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>558</v>
+        <v>571</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>250</v>
+        <v>281</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>395</v>
+        <v>667</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>623</v>
+        <v>668</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>396</v>
+        <v>378</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>622</v>
+        <v>581</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>394</v>
+        <v>303</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>385</v>
+        <v>618</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A142" s="1" t="s">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>482</v>
+        <v>621</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>80</v>
+        <v>392</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A143" s="1" t="s">
-        <v>374</v>
+        <v>386</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>616</v>
+        <v>558</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>375</v>
+        <v>250</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A144" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A145" s="1" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>632</v>
+        <v>623</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A146" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="B146" s="2"/>
-      <c r="C146" s="1"/>
+        <v>393</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A147" s="1" t="s">
-        <v>730</v>
+        <v>384</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>755</v>
+        <v>385</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>731</v>
+        <v>385</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A148" s="1" t="s">
-        <v>83</v>
+        <v>377</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A149" s="1" t="s">
-        <v>85</v>
+        <v>374</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>485</v>
+        <v>616</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>86</v>
+        <v>375</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A150" s="1" t="s">
-        <v>81</v>
+        <v>389</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>483</v>
+        <v>620</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>82</v>
+        <v>390</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A151" s="1" t="s">
-        <v>79</v>
+        <v>413</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>482</v>
+        <v>632</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>80</v>
+        <v>414</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A152" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>78</v>
-      </c>
+        <v>648</v>
+      </c>
+      <c r="B152" s="2"/>
+      <c r="C152" s="1"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A153" s="1" t="s">
-        <v>357</v>
+        <v>726</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>608</v>
+        <v>751</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>358</v>
+        <v>727</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A154" s="1" t="s">
-        <v>359</v>
+        <v>83</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>609</v>
+        <v>484</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>360</v>
+        <v>84</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A155" s="1" t="s">
-        <v>347</v>
+        <v>85</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>603</v>
+        <v>485</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>348</v>
+        <v>86</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A156" s="1" t="s">
-        <v>351</v>
+        <v>81</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>605</v>
+        <v>483</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>352</v>
+        <v>82</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A157" s="1" t="s">
-        <v>353</v>
+        <v>79</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>606</v>
+        <v>482</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>354</v>
+        <v>80</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A158" s="1" t="s">
-        <v>349</v>
+        <v>77</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>604</v>
+        <v>78</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>350</v>
+        <v>78</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A159" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A160" s="1" t="s">
-        <v>649</v>
+        <v>359</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>587</v>
+        <v>609</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>320</v>
+        <v>360</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A161" s="1" t="s">
-        <v>331</v>
+        <v>347</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>593</v>
+        <v>603</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>332</v>
+        <v>348</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A162" s="1" t="s">
-        <v>329</v>
+        <v>351</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>592</v>
+        <v>605</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>330</v>
+        <v>352</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A163" s="1" t="s">
-        <v>674</v>
+        <v>353</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>599</v>
+        <v>606</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A164" s="1" t="s">
-        <v>675</v>
+        <v>349</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>598</v>
+        <v>604</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A165" s="1" t="s">
-        <v>342</v>
+        <v>355</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>600</v>
+        <v>607</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>343</v>
+        <v>356</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A166" s="1" t="s">
-        <v>345</v>
+        <v>649</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>602</v>
+        <v>587</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>346</v>
+        <v>320</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A167" s="1" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>212</v>
+        <v>332</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A168" s="1" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A169" s="1" t="s">
-        <v>333</v>
+        <v>674</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A170" s="1" t="s">
-        <v>327</v>
+        <v>675</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>591</v>
+        <v>598</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>328</v>
+        <v>340</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A171" s="1" t="s">
-        <v>325</v>
+        <v>342</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>590</v>
+        <v>600</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>326</v>
+        <v>343</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A172" s="1" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>596</v>
+        <v>602</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A173" s="1" t="s">
-        <v>676</v>
+        <v>344</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>339</v>
+        <v>212</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A174" s="1" t="s">
-        <v>323</v>
+        <v>335</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>589</v>
+        <v>595</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A175" s="1" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>588</v>
+        <v>594</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A176" s="1" t="s">
-        <v>200</v>
+        <v>327</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>537</v>
+        <v>591</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>201</v>
+        <v>328</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A177" s="1" t="s">
-        <v>203</v>
+        <v>325</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>538</v>
+        <v>590</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>204</v>
+        <v>326</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A178" s="1" t="s">
-        <v>677</v>
+        <v>337</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>534</v>
+        <v>596</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>195</v>
+        <v>338</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A179" s="1" t="s">
-        <v>198</v>
+        <v>676</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>536</v>
+        <v>597</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>199</v>
+        <v>339</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A180" s="1" t="s">
-        <v>193</v>
+        <v>323</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>533</v>
+        <v>589</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>194</v>
+        <v>324</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A181" s="1" t="s">
-        <v>191</v>
+        <v>321</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>532</v>
+        <v>588</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>192</v>
+        <v>322</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A182" s="1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A183" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>504</v>
+        <v>538</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>126</v>
+        <v>204</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A184" s="1" t="s">
-        <v>93</v>
+        <v>677</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>489</v>
+        <v>534</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>94</v>
+        <v>195</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A185" s="1" t="s">
-        <v>111</v>
+        <v>198</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>498</v>
+        <v>536</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>112</v>
+        <v>199</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A186" s="1" t="s">
-        <v>105</v>
+        <v>193</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>495</v>
+        <v>533</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>106</v>
+        <v>194</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A187" s="1" t="s">
-        <v>97</v>
+        <v>191</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>491</v>
+        <v>532</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>98</v>
+        <v>192</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A188" s="1" t="s">
-        <v>99</v>
+        <v>196</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>492</v>
+        <v>535</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>100</v>
+        <v>197</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A189" s="1" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>493</v>
+        <v>504</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A190" s="1" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>128</v>
+        <v>489</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A191" s="1" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>486</v>
+        <v>498</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A192" s="1" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A193" s="1" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>507</v>
+        <v>491</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A194" s="1" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A195" s="1" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>508</v>
+        <v>493</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A196" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>506</v>
+        <v>128</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A197" s="1" t="s">
-        <v>139</v>
+        <v>87</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>510</v>
+        <v>486</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>140</v>
+        <v>88</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A198" s="1" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A199" s="1" t="s">
-        <v>91</v>
+        <v>133</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>488</v>
+        <v>507</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>92</v>
+        <v>134</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A200" s="1" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>496</v>
+        <v>505</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A201" s="1" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>497</v>
+        <v>508</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A202" s="1" t="s">
-        <v>89</v>
+        <v>131</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>487</v>
+        <v>506</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>90</v>
+        <v>132</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A203" s="1" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>500</v>
+        <v>510</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A204" s="1" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>490</v>
+        <v>509</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A205" s="1" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A206" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A207" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A208" s="1" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>503</v>
+        <v>487</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A209" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>118</v>
+        <v>500</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A210" s="1" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A211" s="1" t="s">
-        <v>678</v>
+        <v>125</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>643</v>
+        <v>504</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>435</v>
+        <v>126</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A212" s="1" t="s">
-        <v>679</v>
+        <v>103</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>642</v>
+        <v>494</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>434</v>
+        <v>104</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A213" s="1" t="s">
-        <v>431</v>
+        <v>121</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>640</v>
+        <v>502</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>432</v>
+        <v>122</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A214" s="1" t="s">
-        <v>429</v>
+        <v>123</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>639</v>
+        <v>503</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>430</v>
+        <v>124</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A215" s="1" t="s">
-        <v>421</v>
+        <v>117</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>636</v>
+        <v>118</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>422</v>
+        <v>118</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A216" s="1" t="s">
-        <v>419</v>
+        <v>113</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>635</v>
+        <v>499</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>420</v>
+        <v>114</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A217" s="1" t="s">
-        <v>423</v>
+        <v>678</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>637</v>
+        <v>643</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>424</v>
+        <v>435</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A218" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A219" s="1" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A220" s="1" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>646</v>
+        <v>639</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A221" s="1" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A222" s="1" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A223" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>671</v>
+        <v>637</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A224" s="1" t="s">
-        <v>417</v>
+        <v>680</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>634</v>
+        <v>641</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>418</v>
+        <v>433</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A225" s="1" t="s">
-        <v>415</v>
+        <v>438</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>633</v>
+        <v>645</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>416</v>
+        <v>439</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A226" s="1" t="s">
-        <v>75</v>
+        <v>440</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>481</v>
+        <v>646</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>76</v>
+        <v>441</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A227" s="1" t="s">
-        <v>73</v>
+        <v>436</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>480</v>
+        <v>644</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>74</v>
+        <v>437</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A228" s="1" t="s">
-        <v>71</v>
+        <v>427</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>657</v>
+        <v>638</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>72</v>
+        <v>428</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A229" s="1" t="s">
-        <v>39</v>
+        <v>425</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>464</v>
+        <v>671</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>40</v>
+        <v>426</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A230" s="1" t="s">
-        <v>37</v>
+        <v>417</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>463</v>
+        <v>634</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>38</v>
+        <v>418</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A231" s="1" t="s">
-        <v>50</v>
+        <v>415</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>469</v>
+        <v>633</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>51</v>
+        <v>416</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A232" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>470</v>
+        <v>481</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A233" s="1" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>471</v>
+        <v>480</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A234" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>465</v>
+        <v>657</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A235" s="1" t="s">
-        <v>683</v>
+        <v>39</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>682</v>
+        <v>464</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>681</v>
+        <v>40</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A236" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A237" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A238" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A239" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A240" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A241" s="1" t="s">
-        <v>45</v>
+        <v>683</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>466</v>
+        <v>682</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A242" s="1" t="s">
-        <v>684</v>
+        <v>46</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>685</v>
+        <v>467</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>687</v>
+        <v>47</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A243" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A244" s="1" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>42</v>
+        <v>473</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A245" s="1" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>462</v>
+        <v>475</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A246" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A247" s="1" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>478</v>
+        <v>466</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>70</v>
+        <v>686</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A248" s="1" t="s">
-        <v>66</v>
+        <v>684</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>449</v>
+        <v>685</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>11</v>
+        <v>687</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A249" s="1" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A250" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>447</v>
+        <v>42</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A251" s="1" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>445</v>
+        <v>462</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A252" s="1" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>446</v>
+        <v>477</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A253" s="1" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>444</v>
+        <v>478</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A254" s="1" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A255" s="1" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>455</v>
+        <v>476</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A256" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A257" s="1" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A258" s="1" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A259" s="1" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A260" s="1" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A261" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A262" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A263" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A264" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A265" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A266" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A267" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A268" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A269" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A270" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A271" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A272" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A273" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B267" s="1" t="s">
+      <c r="B273" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="C267" s="1" t="s">
+      <c r="C273" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor: Refactoring of source code
</commit_message>
<xml_diff>
--- a/gen/properties_list.xlsx
+++ b/gen/properties_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="778">
   <si>
     <t>wizard.new.erd.title</t>
   </si>
@@ -2484,6 +2484,18 @@
   </si>
   <si>
     <t>html.column.notNull</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>参照キーとして利用できるカラムがありません</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>No column available as reference key</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>error.select.referenceKey</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2602,10 +2614,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="テーブル2" displayName="テーブル2" ref="A2:C273" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A2:C273"/>
-  <sortState ref="A3:C273">
-    <sortCondition ref="A2:A273"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="テーブル2" displayName="テーブル2" ref="A2:C274" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A2:C274"/>
+  <sortState ref="A3:C274">
+    <sortCondition ref="A2:A274"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="2" name="Key" dataDxfId="2"/>
@@ -2903,9 +2915,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C273"/>
+  <dimension ref="A2:C274"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4060,1845 +4074,1856 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A106" s="1" t="s">
-        <v>369</v>
+        <v>777</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>614</v>
+        <v>776</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>370</v>
+        <v>775</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>773</v>
+        <v>369</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>771</v>
+        <v>614</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>772</v>
+        <v>370</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
-        <v>770</v>
+        <v>773</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>744</v>
+        <v>771</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>699</v>
+        <v>772</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>717</v>
+        <v>770</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>730</v>
+        <v>744</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>745</v>
+        <v>730</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
-        <v>713</v>
+        <v>718</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>740</v>
+        <v>745</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>693</v>
+        <v>701</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
-        <v>774</v>
+        <v>713</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
-        <v>714</v>
+        <v>774</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>738</v>
+        <v>714</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>752</v>
+        <v>694</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
-        <v>712</v>
+        <v>738</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>692</v>
+        <v>752</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>732</v>
+        <v>742</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
-        <v>764</v>
+        <v>716</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
-        <v>722</v>
+        <v>764</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>749</v>
+        <v>734</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A121" s="1" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>731</v>
+        <v>748</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>747</v>
+        <v>731</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
-        <v>762</v>
+        <v>719</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>755</v>
+        <v>746</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>756</v>
+        <v>702</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>767</v>
+        <v>755</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>765</v>
+        <v>756</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>757</v>
+        <v>765</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
-        <v>759</v>
+        <v>769</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>760</v>
+        <v>768</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>753</v>
+        <v>760</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>754</v>
+        <v>761</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>725</v>
+        <v>763</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>708</v>
+        <v>754</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
-        <v>711</v>
+        <v>725</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>736</v>
+        <v>750</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>691</v>
+        <v>708</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>729</v>
+        <v>736</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
-        <v>758</v>
+        <v>710</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>728</v>
+        <v>735</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A135" s="1" t="s">
-        <v>373</v>
+        <v>758</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>670</v>
+        <v>728</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>669</v>
+        <v>688</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
-        <v>665</v>
+        <v>373</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>376</v>
+        <v>669</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A137" s="1" t="s">
-        <v>397</v>
+        <v>665</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>571</v>
+        <v>666</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>281</v>
+        <v>376</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
-        <v>379</v>
+        <v>397</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>617</v>
+        <v>571</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>380</v>
+        <v>281</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>667</v>
+        <v>379</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>668</v>
+        <v>617</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
-        <v>381</v>
+        <v>667</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>581</v>
+        <v>668</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>303</v>
+        <v>378</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>618</v>
+        <v>581</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>383</v>
+        <v>303</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A142" s="1" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A143" s="1" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>558</v>
+        <v>621</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>250</v>
+        <v>392</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A144" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>619</v>
+        <v>558</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>388</v>
+        <v>250</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A145" s="1" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A146" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A147" s="1" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>385</v>
+        <v>622</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A148" s="1" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>482</v>
+        <v>385</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>80</v>
+        <v>385</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A149" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>616</v>
+        <v>482</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>375</v>
+        <v>80</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A150" s="1" t="s">
-        <v>389</v>
+        <v>374</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>390</v>
+        <v>375</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A151" s="1" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>632</v>
+        <v>620</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>414</v>
+        <v>390</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A152" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="B152" s="2"/>
-      <c r="C152" s="1"/>
+        <v>413</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A153" s="1" t="s">
-        <v>726</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>751</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>727</v>
-      </c>
+        <v>648</v>
+      </c>
+      <c r="B153" s="2"/>
+      <c r="C153" s="1"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A154" s="1" t="s">
-        <v>83</v>
+        <v>726</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>484</v>
+        <v>751</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>84</v>
+        <v>727</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A155" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A156" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A157" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A158" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>78</v>
+        <v>482</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A159" s="1" t="s">
-        <v>357</v>
+        <v>77</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>608</v>
+        <v>78</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>358</v>
+        <v>78</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A160" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A161" s="1" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>603</v>
+        <v>609</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A162" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A163" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A164" s="1" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A165" s="1" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A166" s="1" t="s">
-        <v>649</v>
+        <v>355</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>587</v>
+        <v>607</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>320</v>
+        <v>356</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A167" s="1" t="s">
-        <v>331</v>
+        <v>649</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A168" s="1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A169" s="1" t="s">
-        <v>674</v>
+        <v>329</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A170" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A171" s="1" t="s">
-        <v>342</v>
+        <v>675</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A172" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A173" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>212</v>
+        <v>346</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A174" s="1" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>595</v>
+        <v>601</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>336</v>
+        <v>212</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A175" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A176" s="1" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A177" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A178" s="1" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A179" s="1" t="s">
-        <v>676</v>
+        <v>337</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A180" s="1" t="s">
-        <v>323</v>
+        <v>676</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>589</v>
+        <v>597</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>324</v>
+        <v>339</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A181" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A182" s="1" t="s">
-        <v>200</v>
+        <v>321</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>537</v>
+        <v>588</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>201</v>
+        <v>322</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A183" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A184" s="1" t="s">
-        <v>677</v>
+        <v>203</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A185" s="1" t="s">
-        <v>198</v>
+        <v>677</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A186" s="1" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A187" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A188" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A189" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>504</v>
+        <v>535</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>126</v>
+        <v>197</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A190" s="1" t="s">
-        <v>93</v>
+        <v>202</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>489</v>
+        <v>504</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A191" s="1" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A192" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A193" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A194" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A195" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A196" s="1" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>128</v>
+        <v>493</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A197" s="1" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>486</v>
+        <v>128</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A198" s="1" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>501</v>
+        <v>486</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A199" s="1" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A200" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A201" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A202" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A203" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A204" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A205" s="1" t="s">
-        <v>91</v>
+        <v>137</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>488</v>
+        <v>509</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>92</v>
+        <v>138</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A206" s="1" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A207" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A208" s="1" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>487</v>
+        <v>497</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A209" s="1" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A210" s="1" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>490</v>
+        <v>500</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A211" s="1" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A212" s="1" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>494</v>
+        <v>504</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A213" s="1" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A214" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A215" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>118</v>
+        <v>503</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A216" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>499</v>
+        <v>118</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A217" s="1" t="s">
-        <v>678</v>
+        <v>113</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>643</v>
+        <v>499</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>435</v>
+        <v>114</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A218" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A219" s="1" t="s">
-        <v>431</v>
+        <v>679</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A220" s="1" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A221" s="1" t="s">
-        <v>421</v>
+        <v>429</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>422</v>
+        <v>430</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A222" s="1" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A223" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A224" s="1" t="s">
-        <v>680</v>
+        <v>423</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A225" s="1" t="s">
-        <v>438</v>
+        <v>680</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A226" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A227" s="1" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A228" s="1" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>638</v>
+        <v>644</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A229" s="1" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>671</v>
+        <v>638</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A230" s="1" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>634</v>
+        <v>671</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>418</v>
+        <v>426</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A231" s="1" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A232" s="1" t="s">
-        <v>75</v>
+        <v>415</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>481</v>
+        <v>633</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>76</v>
+        <v>416</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A233" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A234" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>657</v>
+        <v>480</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A235" s="1" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>464</v>
+        <v>657</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A236" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A237" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A238" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A239" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A240" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A241" s="1" t="s">
-        <v>683</v>
+        <v>43</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>682</v>
+        <v>465</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>681</v>
+        <v>44</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A242" s="1" t="s">
-        <v>46</v>
+        <v>683</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>467</v>
+        <v>682</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>47</v>
+        <v>681</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A243" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A244" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A245" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A246" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A247" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>686</v>
+        <v>57</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A248" s="1" t="s">
-        <v>684</v>
+        <v>45</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>685</v>
+        <v>466</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A249" s="1" t="s">
-        <v>48</v>
+        <v>684</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>468</v>
+        <v>685</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>49</v>
+        <v>687</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A250" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>42</v>
+        <v>468</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A251" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>462</v>
+        <v>42</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A252" s="1" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A253" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A254" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>449</v>
+        <v>478</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A255" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>476</v>
+        <v>449</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>65</v>
+        <v>11</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A256" s="1" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>447</v>
+        <v>476</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A257" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A258" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A259" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A260" s="1" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>461</v>
+        <v>444</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A261" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>455</v>
+        <v>461</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A262" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A263" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A264" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A265" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A266" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A267" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A268" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A269" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A270" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>448</v>
+        <v>458</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A271" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A272" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A273" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A274" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B273" s="1" t="s">
+      <c r="B274" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="C273" s="1" t="s">
+      <c r="C274" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: Fixed a bug in the import process.
</commit_message>
<xml_diff>
--- a/gen/properties_list.xlsx
+++ b/gen/properties_list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="781">
   <si>
     <t>wizard.new.erd.title</t>
   </si>
@@ -2498,6 +2498,18 @@
   </si>
   <si>
     <t>キー重複エラー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wizard.new.import.database</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Database</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>データベース</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2616,8 +2628,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="テーブル2" displayName="テーブル2" ref="A2:C274" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A2:C274"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="テーブル2" displayName="テーブル2" ref="A2:C275" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A2:C275"/>
   <sortState ref="A3:C274">
     <sortCondition ref="A2:A274"/>
   </sortState>
@@ -2917,7 +2929,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C274"/>
+  <dimension ref="A2:C275"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5797,133 +5809,144 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A263" s="1" t="s">
-        <v>12</v>
+        <v>778</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>449</v>
+        <v>779</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>13</v>
+        <v>780</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A264" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A265" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A266" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A267" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A268" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A269" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A270" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A271" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A272" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A273" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A274" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A275" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B274" s="1" t="s">
+      <c r="B275" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="C274" s="1" t="s">
+      <c r="C275" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update: Modification of HTML output content.
</commit_message>
<xml_diff>
--- a/gen/properties_list.xlsx
+++ b/gen/properties_list.xlsx
@@ -11,14 +11,13 @@
     <sheet name="MESSAGE" sheetId="6" r:id="rId2"/>
     <sheet name="VALIDATE" sheetId="5" r:id="rId3"/>
     <sheet name="TYPE" sheetId="3" r:id="rId4"/>
-    <sheet name="HTML" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="651">
   <si>
     <t>物理名を自動的に論理名に変換する（日本語のみ）</t>
   </si>
@@ -1125,332 +1124,6 @@
   </si>
   <si>
     <t>Line separator</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テーブル定義</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>論理テーブル名</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>説明</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>No.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>論理名</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>物理名</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>型</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>必須</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>一意</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>符号無し</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>初期値</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>備考</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ドメイン</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>インデックス</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>外部キー</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ドメイン定義</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ドメイン名</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>サイズ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>このテーブルを参照しているテーブル</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.table.logicalName</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.table.physicalName</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.table.description</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.column.rownum</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.column.logicalName</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.column.physicalName</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.column.type</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.column.unique</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.column.description</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.column.description.domain</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.indices</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.foreignKeys</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.domain.title</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.domain.name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.domain.type</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.domain.size</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.referencedTables</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Tables</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Logical Table Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Unique</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Unsigned</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Domain Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Physical Table Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.column.primaryKey</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PrimaryKey</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Logical Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Physical Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Not Null</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Default Value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Domain</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Indices</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Foreign Keys</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Domain Definitions</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Size</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Referenced Tables</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>主キー</t>
-    <rPh sb="0" eb="1">
-      <t>シュ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Table</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テーブル</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Attribute Overview</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>属性の概要</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>外部キー</t>
-    <rPh sb="0" eb="2">
-      <t>ガイブ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.title</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.page.section.title.index</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Indexing Overview</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>インデックスの概要</t>
-    <rPh sb="7" eb="9">
-      <t>ガイヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.page.section.title.attribute</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.page.title.table</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.column.unsigned</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>複合一意キー</t>
-    <rPh sb="0" eb="2">
-      <t>フクゴウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>イチイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.page.section.title.compositeUniqueKeys</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Composite Unique Keys</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.page.section.title.foreignKeys</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.column.defaultValue</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Auto Increment</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>自動採番</t>
-    <rPh sb="2" eb="4">
-      <t>サイバン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.column.autoIncrement</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>html.column.notNull</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -2866,55 +2539,7 @@
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -3121,26 +2746,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="テーブル22" displayName="テーブル22" ref="A2:D152" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="テーブル22" displayName="テーブル22" ref="A2:D152" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A2:D152"/>
   <sortState ref="A3:D152">
     <sortCondition ref="A2:A152"/>
-  </sortState>
-  <tableColumns count="4">
-    <tableColumn id="2" name="Key" dataDxfId="27"/>
-    <tableColumn id="3" name="English" dataDxfId="26"/>
-    <tableColumn id="4" name="Japanese" dataDxfId="25"/>
-    <tableColumn id="1" name="備考" dataDxfId="24"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="テーブル227" displayName="テーブル227" ref="A2:D18" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A2:D18"/>
-  <sortState ref="A3:D18">
-    <sortCondition ref="A2:A18"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="2" name="Key" dataDxfId="21"/>
@@ -3152,11 +2761,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="テーブル226" displayName="テーブル226" ref="A2:D17" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A2:D17"/>
-  <sortState ref="A3:D248">
-    <sortCondition ref="A2:A248"/>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="テーブル227" displayName="テーブル227" ref="A2:D18" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A2:D18"/>
+  <sortState ref="A3:D18">
+    <sortCondition ref="A2:A18"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="2" name="Key" dataDxfId="15"/>
@@ -3168,11 +2777,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="テーブル224" displayName="テーブル224" ref="A2:D30" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A2:D30"/>
-  <sortState ref="A3:D30">
-    <sortCondition ref="A2:A30"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="テーブル226" displayName="テーブル226" ref="A2:D17" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A2:D17"/>
+  <sortState ref="A3:D248">
+    <sortCondition ref="A2:A248"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="2" name="Key" dataDxfId="9"/>
@@ -3184,11 +2793,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="テーブル225" displayName="テーブル225" ref="A2:D30" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="テーブル224" displayName="テーブル224" ref="A2:D30" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A2:D30"/>
-  <sortState ref="A3:D248">
-    <sortCondition ref="A2:A248"/>
+  <sortState ref="A3:D30">
+    <sortCondition ref="A2:A30"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="2" name="Key" dataDxfId="3"/>
@@ -3510,7 +3119,7 @@
         <v>217</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>450</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3524,7 +3133,7 @@
         <v>81</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3538,7 +3147,7 @@
         <v>101</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3552,7 +3161,7 @@
         <v>95</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3566,7 +3175,7 @@
         <v>75</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -3580,7 +3189,7 @@
         <v>83</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3594,7 +3203,7 @@
         <v>77</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -3608,7 +3217,7 @@
         <v>91</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -3622,7 +3231,7 @@
         <v>93</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3636,7 +3245,7 @@
         <v>97</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3650,7 +3259,7 @@
         <v>79</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3664,7 +3273,7 @@
         <v>104</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3678,7 +3287,7 @@
         <v>99</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3692,7 +3301,7 @@
         <v>73</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3706,7 +3315,7 @@
         <v>350</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3720,7 +3329,7 @@
         <v>85</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3734,7 +3343,7 @@
         <v>87</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3748,54 +3357,54 @@
         <v>89</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>621</v>
+        <v>544</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>613</v>
+        <v>536</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>615</v>
+        <v>538</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>619</v>
+        <v>542</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>622</v>
+        <v>545</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>616</v>
+        <v>539</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>617</v>
+        <v>540</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>620</v>
+        <v>543</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>622</v>
+        <v>545</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>612</v>
+        <v>535</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>614</v>
+        <v>537</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>618</v>
+        <v>541</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>622</v>
+        <v>545</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>607</v>
+        <v>530</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>282</v>
@@ -3804,7 +3413,7 @@
         <v>115</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>683</v>
+        <v>606</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -3818,7 +3427,7 @@
         <v>113</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>682</v>
+        <v>605</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -3826,13 +3435,13 @@
         <v>136</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>668</v>
+        <v>591</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>610</v>
+        <v>533</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>666</v>
+        <v>589</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -3840,41 +3449,41 @@
         <v>134</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>667</v>
+        <v>590</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>608</v>
+        <v>531</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>665</v>
+        <v>588</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>660</v>
+        <v>583</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>663</v>
+        <v>586</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>661</v>
+        <v>584</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>664</v>
+        <v>587</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>687</v>
+        <v>610</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>686</v>
+        <v>609</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>685</v>
+        <v>608</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>684</v>
+        <v>607</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3885,10 +3494,10 @@
         <v>281</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>670</v>
+        <v>593</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>669</v>
+        <v>592</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3902,7 +3511,7 @@
         <v>120</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>672</v>
+        <v>595</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -3913,24 +3522,24 @@
         <v>284</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>674</v>
+        <v>597</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>671</v>
+        <v>594</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>693</v>
+        <v>616</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>691</v>
+        <v>614</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>691</v>
+        <v>614</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>692</v>
+        <v>615</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -3938,18 +3547,18 @@
         <v>122</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>662</v>
+        <v>585</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>609</v>
+        <v>532</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>673</v>
+        <v>596</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>547</v>
+        <v>470</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>331</v>
@@ -3958,7 +3567,7 @@
         <v>187</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -3972,7 +3581,7 @@
         <v>173</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -3986,12 +3595,12 @@
         <v>133</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>548</v>
+        <v>471</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>330</v>
@@ -4000,35 +3609,35 @@
         <v>186</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>530</v>
+        <v>453</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>527</v>
+        <v>450</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>493</v>
+        <v>416</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>524</v>
+        <v>447</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>224</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>523</v>
+        <v>446</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -4042,12 +3651,12 @@
         <v>176</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>538</v>
+        <v>461</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>291</v>
@@ -4056,12 +3665,12 @@
         <v>125</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>537</v>
+        <v>460</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>290</v>
@@ -4070,54 +3679,54 @@
         <v>124</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>522</v>
+        <v>445</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>447</v>
+        <v>370</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>448</v>
+        <v>371</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>535</v>
+        <v>458</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>504</v>
+        <v>427</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>482</v>
+        <v>405</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>536</v>
+        <v>459</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>505</v>
+        <v>428</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>483</v>
+        <v>406</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
-        <v>549</v>
+        <v>472</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>333</v>
@@ -4126,7 +3735,7 @@
         <v>189</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -4140,7 +3749,7 @@
         <v>174</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -4154,26 +3763,26 @@
         <v>135</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>611</v>
+        <v>534</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>499</v>
+        <v>422</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>477</v>
+        <v>400</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>553</v>
+        <v>476</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>295</v>
@@ -4182,12 +3791,12 @@
         <v>129</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>550</v>
+        <v>473</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>332</v>
@@ -4196,12 +3805,12 @@
         <v>188</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>555</v>
+        <v>478</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>296</v>
@@ -4210,26 +3819,26 @@
         <v>130</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>556</v>
+        <v>479</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>506</v>
+        <v>429</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>484</v>
+        <v>407</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
-        <v>648</v>
+        <v>571</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>311</v>
@@ -4238,26 +3847,26 @@
         <v>147</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
-        <v>526</v>
+        <v>449</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>223</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>490</v>
+        <v>413</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
-        <v>534</v>
+        <v>457</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>277</v>
@@ -4266,26 +3875,26 @@
         <v>107</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
-        <v>545</v>
+        <v>468</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>449</v>
+        <v>372</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>449</v>
+        <v>372</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
-        <v>546</v>
+        <v>469</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>313</v>
@@ -4294,7 +3903,7 @@
         <v>148</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -4308,124 +3917,124 @@
         <v>179</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
-        <v>676</v>
+        <v>599</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>299</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>675</v>
+        <v>598</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
-        <v>558</v>
+        <v>481</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>510</v>
+        <v>433</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>487</v>
+        <v>410</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
-        <v>559</v>
+        <v>482</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>511</v>
+        <v>434</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>488</v>
+        <v>411</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
-        <v>544</v>
+        <v>467</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>529</v>
+        <v>452</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>495</v>
+        <v>418</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
-        <v>531</v>
+        <v>454</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>528</v>
+        <v>451</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>494</v>
+        <v>417</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="1" t="s">
-        <v>532</v>
+        <v>455</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>515</v>
+        <v>438</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>498</v>
+        <v>421</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="1" t="s">
-        <v>525</v>
+        <v>448</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>364</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>491</v>
+        <v>414</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="1" t="s">
-        <v>541</v>
+        <v>464</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>507</v>
+        <v>430</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>485</v>
+        <v>408</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="1" t="s">
-        <v>539</v>
+        <v>462</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>276</v>
@@ -4434,12 +4043,12 @@
         <v>106</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="1" t="s">
-        <v>677</v>
+        <v>600</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>285</v>
@@ -4448,12 +4057,12 @@
         <v>118</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="1" t="s">
-        <v>678</v>
+        <v>601</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>288</v>
@@ -4462,7 +4071,7 @@
         <v>121</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -4476,63 +4085,63 @@
         <v>126</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="1" t="s">
-        <v>451</v>
+        <v>374</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>456</v>
+        <v>379</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>454</v>
+        <v>377</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="1" t="s">
-        <v>679</v>
+        <v>602</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>501</v>
+        <v>424</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>479</v>
+        <v>402</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="1" t="s">
-        <v>680</v>
+        <v>603</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>502</v>
+        <v>425</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>480</v>
+        <v>403</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="1" t="s">
-        <v>474</v>
+        <v>397</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>475</v>
+        <v>398</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>476</v>
+        <v>399</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -4546,21 +4155,21 @@
         <v>184</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="1" t="s">
-        <v>521</v>
+        <v>444</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>512</v>
+        <v>435</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>496</v>
+        <v>419</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -4574,12 +4183,12 @@
         <v>182</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="1" t="s">
-        <v>540</v>
+        <v>463</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>275</v>
@@ -4588,12 +4197,12 @@
         <v>105</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="1" t="s">
-        <v>542</v>
+        <v>465</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>289</v>
@@ -4602,77 +4211,77 @@
         <v>123</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="1" t="s">
-        <v>681</v>
+        <v>604</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>503</v>
+        <v>426</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>481</v>
+        <v>404</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="1" t="s">
-        <v>519</v>
+        <v>442</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>513</v>
+        <v>436</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>497</v>
+        <v>420</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="1" t="s">
-        <v>557</v>
+        <v>480</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>500</v>
+        <v>423</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>486</v>
+        <v>409</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="1" t="s">
-        <v>520</v>
+        <v>443</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>514</v>
+        <v>437</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>489</v>
+        <v>412</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="1" t="s">
-        <v>551</v>
+        <v>474</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>508</v>
+        <v>431</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>478</v>
+        <v>401</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -4686,12 +4295,12 @@
         <v>172</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="1" t="s">
-        <v>543</v>
+        <v>466</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>293</v>
@@ -4700,26 +4309,26 @@
         <v>127</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="1" t="s">
-        <v>552</v>
+        <v>475</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>509</v>
+        <v>432</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>132</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="1" t="s">
-        <v>533</v>
+        <v>456</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>297</v>
@@ -4728,12 +4337,12 @@
         <v>131</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="1" t="s">
-        <v>554</v>
+        <v>477</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>294</v>
@@ -4742,40 +4351,40 @@
         <v>128</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="1" t="s">
-        <v>516</v>
+        <v>439</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>517</v>
+        <v>440</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>518</v>
+        <v>441</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="1" t="s">
-        <v>689</v>
+        <v>612</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>688</v>
+        <v>611</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>690</v>
+        <v>613</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="1" t="s">
-        <v>649</v>
+        <v>572</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>312</v>
@@ -4784,63 +4393,63 @@
         <v>115</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="1" t="s">
-        <v>452</v>
+        <v>375</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>453</v>
+        <v>376</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>455</v>
+        <v>378</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>632</v>
+        <v>555</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="1" t="s">
-        <v>715</v>
+        <v>638</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>718</v>
+        <v>641</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>719</v>
+        <v>642</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>724</v>
+        <v>647</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="1" t="s">
-        <v>717</v>
+        <v>640</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>722</v>
+        <v>645</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>723</v>
+        <v>646</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>724</v>
+        <v>647</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="1" t="s">
-        <v>716</v>
+        <v>639</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>720</v>
+        <v>643</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>721</v>
+        <v>644</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>724</v>
+        <v>647</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -4862,7 +4471,7 @@
         <v>15</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>633</v>
+        <v>556</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -4876,7 +4485,7 @@
         <v>17</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>633</v>
+        <v>556</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -4890,7 +4499,7 @@
         <v>13</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>633</v>
+        <v>556</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -4904,7 +4513,7 @@
         <v>11</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>633</v>
+        <v>556</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -4915,10 +4524,10 @@
         <v>9</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>560</v>
+        <v>483</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>633</v>
+        <v>556</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -4932,7 +4541,7 @@
         <v>160</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -4946,7 +4555,7 @@
         <v>162</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -4960,7 +4569,7 @@
         <v>150</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -4974,7 +4583,7 @@
         <v>154</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -4988,7 +4597,7 @@
         <v>156</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -5002,7 +4611,7 @@
         <v>152</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -5016,12 +4625,12 @@
         <v>158</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="1" t="s">
-        <v>650</v>
+        <v>573</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>301</v>
@@ -5030,12 +4639,12 @@
         <v>137</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="1" t="s">
-        <v>651</v>
+        <v>574</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>310</v>
@@ -5044,12 +4653,12 @@
         <v>146</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="1" t="s">
-        <v>652</v>
+        <v>575</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>309</v>
@@ -5058,12 +4667,12 @@
         <v>145</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="1" t="s">
-        <v>653</v>
+        <v>576</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>306</v>
@@ -5072,12 +4681,12 @@
         <v>142</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="1" t="s">
-        <v>654</v>
+        <v>577</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>305</v>
@@ -5086,12 +4695,12 @@
         <v>141</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="1" t="s">
-        <v>655</v>
+        <v>578</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>304</v>
@@ -5100,12 +4709,12 @@
         <v>140</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="1" t="s">
-        <v>656</v>
+        <v>579</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>303</v>
@@ -5114,12 +4723,12 @@
         <v>139</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="1" t="s">
-        <v>657</v>
+        <v>580</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>307</v>
@@ -5128,12 +4737,12 @@
         <v>143</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="1" t="s">
-        <v>658</v>
+        <v>581</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>308</v>
@@ -5142,12 +4751,12 @@
         <v>144</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="1" t="s">
-        <v>659</v>
+        <v>582</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>302</v>
@@ -5156,7 +4765,7 @@
         <v>138</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>634</v>
+        <v>557</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -5170,7 +4779,7 @@
         <v>109</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>635</v>
+        <v>558</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -5184,12 +4793,12 @@
         <v>111</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>635</v>
+        <v>558</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="1" t="s">
-        <v>629</v>
+        <v>552</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>254</v>
@@ -5198,68 +4807,68 @@
         <v>57</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>635</v>
+        <v>558</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="3" t="s">
-        <v>590</v>
+        <v>513</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>601</v>
+        <v>524</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>457</v>
+        <v>380</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>636</v>
+        <v>559</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="3" t="s">
-        <v>458</v>
+        <v>381</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>468</v>
+        <v>391</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>636</v>
+        <v>559</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="3" t="s">
-        <v>459</v>
+        <v>382</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>593</v>
+        <v>516</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>457</v>
+        <v>380</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>636</v>
+        <v>559</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="4" t="s">
-        <v>631</v>
+        <v>554</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>628</v>
+        <v>551</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>492</v>
+        <v>415</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>641</v>
+        <v>564</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
-        <v>624</v>
+        <v>547</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>226</v>
@@ -5268,12 +4877,12 @@
         <v>2</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>637</v>
+        <v>560</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="4" t="s">
-        <v>626</v>
+        <v>549</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>227</v>
@@ -5282,12 +4891,12 @@
         <v>3</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>637</v>
+        <v>560</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="4" t="s">
-        <v>630</v>
+        <v>553</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>363</v>
@@ -5296,12 +4905,12 @@
         <v>362</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>637</v>
+        <v>560</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="4" t="s">
-        <v>625</v>
+        <v>548</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>225</v>
@@ -5310,180 +4919,180 @@
         <v>1</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>638</v>
+        <v>561</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="3" t="s">
-        <v>594</v>
+        <v>517</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>598</v>
+        <v>521</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>595</v>
+        <v>518</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>638</v>
+        <v>561</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="3" t="s">
-        <v>467</v>
+        <v>390</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>591</v>
+        <v>514</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>592</v>
+        <v>515</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>637</v>
+        <v>560</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="3" t="s">
-        <v>460</v>
+        <v>383</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>602</v>
+        <v>525</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>603</v>
+        <v>526</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>639</v>
+        <v>562</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="4" t="s">
-        <v>589</v>
+        <v>512</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>599</v>
+        <v>522</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>606</v>
+        <v>529</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>640</v>
+        <v>563</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="3" t="s">
-        <v>466</v>
+        <v>389</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>583</v>
+        <v>506</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>581</v>
+        <v>504</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>640</v>
+        <v>563</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="4" t="s">
-        <v>461</v>
+        <v>384</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>584</v>
+        <v>507</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>582</v>
+        <v>505</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>640</v>
+        <v>563</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="3" t="s">
-        <v>588</v>
+        <v>511</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>579</v>
+        <v>502</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>604</v>
+        <v>527</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>642</v>
+        <v>565</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="3" t="s">
-        <v>462</v>
+        <v>385</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>580</v>
+        <v>503</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>577</v>
+        <v>500</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>643</v>
+        <v>566</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="4" t="s">
-        <v>463</v>
+        <v>386</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>585</v>
+        <v>508</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>578</v>
+        <v>501</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>643</v>
+        <v>566</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="4" t="s">
-        <v>627</v>
+        <v>550</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>600</v>
+        <v>523</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>605</v>
+        <v>528</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>644</v>
+        <v>567</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="4" t="s">
-        <v>470</v>
+        <v>393</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>576</v>
+        <v>499</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>575</v>
+        <v>498</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>644</v>
+        <v>567</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="4" t="s">
-        <v>469</v>
+        <v>392</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>471</v>
+        <v>394</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>472</v>
+        <v>395</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>644</v>
+        <v>567</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="4" t="s">
-        <v>623</v>
+        <v>546</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>222</v>
@@ -5492,119 +5101,119 @@
         <v>0</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>645</v>
+        <v>568</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="3" t="s">
-        <v>586</v>
+        <v>509</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>220</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>596</v>
+        <v>519</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>645</v>
+        <v>568</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="3" t="s">
-        <v>564</v>
+        <v>487</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>571</v>
+        <v>494</v>
       </c>
       <c r="C146" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="D146" s="1" t="s">
         <v>569</v>
-      </c>
-      <c r="D146" s="1" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="3" t="s">
-        <v>565</v>
+        <v>488</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>570</v>
+        <v>493</v>
       </c>
       <c r="C147" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="D147" s="1" t="s">
         <v>568</v>
-      </c>
-      <c r="D147" s="1" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="4" t="s">
-        <v>566</v>
+        <v>489</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>221</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>573</v>
+        <v>496</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>645</v>
+        <v>568</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="4" t="s">
-        <v>567</v>
+        <v>490</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>574</v>
+        <v>497</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>572</v>
+        <v>495</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>645</v>
+        <v>568</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="3" t="s">
-        <v>587</v>
+        <v>510</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>473</v>
+        <v>396</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>597</v>
+        <v>520</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="3" t="s">
-        <v>464</v>
+        <v>387</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>561</v>
+        <v>484</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>562</v>
+        <v>485</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="3" t="s">
-        <v>465</v>
+        <v>388</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>219</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>563</v>
+        <v>486</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>647</v>
+        <v>570</v>
       </c>
     </row>
   </sheetData>
@@ -5642,18 +5251,18 @@
         <v>217</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>450</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>711</v>
+        <v>634</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>712</v>
+        <v>635</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>713</v>
+        <v>636</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -5665,13 +5274,13 @@
         <v>323</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>714</v>
+        <v>637</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>695</v>
+        <v>618</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>283</v>
@@ -5683,7 +5292,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>696</v>
+        <v>619</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>286</v>
@@ -5707,13 +5316,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>710</v>
+        <v>633</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>708</v>
+        <v>631</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>709</v>
+        <v>632</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -5722,10 +5331,10 @@
         <v>170</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>445</v>
+        <v>368</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>446</v>
+        <v>369</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -5743,13 +5352,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>444</v>
+        <v>367</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>443</v>
+        <v>366</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>442</v>
+        <v>365</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -5767,7 +5376,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>698</v>
+        <v>621</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>229</v>
@@ -5779,7 +5388,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>699</v>
+        <v>622</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>228</v>
@@ -5791,7 +5400,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>697</v>
+        <v>620</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>230</v>
@@ -5803,37 +5412,37 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>702</v>
+        <v>625</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>700</v>
+        <v>623</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>701</v>
+        <v>624</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>707</v>
+        <v>630</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>706</v>
+        <v>629</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>694</v>
+        <v>617</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>704</v>
+        <v>627</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>703</v>
+        <v>626</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>705</v>
+        <v>628</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -5872,7 +5481,7 @@
         <v>217</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>450</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6090,7 +5699,7 @@
         <v>217</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>450</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6167,13 +5776,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>725</v>
+        <v>648</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>726</v>
+        <v>649</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>727</v>
+        <v>650</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -6426,380 +6035,6 @@
       </c>
       <c r="C30" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D30" s="1"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="45.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.375" customWidth="1"/>
-    <col min="3" max="3" width="66.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>365</v>
       </c>
       <c r="D30" s="1"/>
     </row>

</xml_diff>